<commit_message>
ARKCORR-18 Added bussiness process definitions for the on enter queue rule.
</commit_message>
<xml_diff>
--- a/acm/rules/drools-on-enter-queue-rules-correspondence.xlsx
+++ b/acm/rules/drools-on-enter-queue-rules-correspondence.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="16925"/>
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lazo.lazarev\Documents\ACM3\acm-plugins\acm-default-plugins\acm-case-file-plugin\src\main\resources\rules\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lazo.lazarev\.arkcase\acm\rules\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -76,7 +76,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="41">
   <si>
     <t>RuleSet</t>
   </si>
@@ -132,22 +132,10 @@
     <t>Functions</t>
   </si>
   <si>
-    <t>eval(evalSpring("$param", $model))</t>
-  </si>
-  <si>
-    <t>Arbitrary rule, as for now we want to rule to always evaluate to true.</t>
-  </si>
-  <si>
     <t>com.armedia.acm.plugins.businessprocess.model.OnEnterQueueModel</t>
   </si>
   <si>
     <t>$model: OnEnterQueueModel</t>
-  </si>
-  <si>
-    <t>$model.setBusinessProcessName($param);</t>
-  </si>
-  <si>
-    <t>The business process to be executed in case rules are satisfied</t>
   </si>
   <si>
     <t>function Boolean evalSpring(String expression, OnEnterQueueModel model)
@@ -161,20 +149,71 @@
 }</t>
   </si>
   <si>
-    <t>enqueueName.equals("next-queue")</t>
-  </si>
-  <si>
     <t>com.armedia.acm.plugins.casefile.pipeline.CaseFilePipelineContext</t>
+  </si>
+  <si>
+    <t>((CaseFilePipelineContext) $model.getPipelineContext()).getEnqueueName().equals("$param")</t>
+  </si>
+  <si>
+    <t>$model.setBusinessProcessName("$param");</t>
+  </si>
+  <si>
+    <t>Entering Queue Name</t>
+  </si>
+  <si>
+    <t>The business process to be executed when entering that queue</t>
+  </si>
+  <si>
+    <t>Fulfill queue</t>
+  </si>
+  <si>
+    <t>Fulfill</t>
+  </si>
+  <si>
+    <t>Intake queue</t>
+  </si>
+  <si>
+    <t>Supervisor Approval queue</t>
+  </si>
+  <si>
+    <t>Executive Approval queue</t>
+  </si>
+  <si>
+    <t>Release queue</t>
+  </si>
+  <si>
+    <t>Intake</t>
+  </si>
+  <si>
+    <t>Supervisor Approval</t>
+  </si>
+  <si>
+    <t>Executive Approval</t>
+  </si>
+  <si>
+    <t>Release</t>
+  </si>
+  <si>
+    <t>correspondence-extension-intake-process</t>
+  </si>
+  <si>
+    <t>correspondence-extension-fulfill-process</t>
+  </si>
+  <si>
+    <t>correspondence-extension-executive-approval-process</t>
+  </si>
+  <si>
+    <t>correspondence-extension-supervisor-approval-process</t>
+  </si>
+  <si>
+    <t>correspondence-extension-release-process</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
-  </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -196,12 +235,6 @@
       <name val="Tahoma"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="9">
@@ -254,7 +287,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -408,24 +441,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyProtection="1"/>
@@ -452,12 +472,6 @@
       <alignment wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
@@ -466,7 +480,7 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1029,10 +1043,10 @@
   <sheetPr>
     <tabColor rgb="FFFFFFFF"/>
   </sheetPr>
-  <dimension ref="A1:G20"/>
+  <dimension ref="A1:G23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" topLeftCell="C16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1076,7 +1090,7 @@
         <v>2</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
@@ -1085,10 +1099,10 @@
     <row r="4" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
-      <c r="C4" s="20" t="s">
+      <c r="C4" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="21" t="s">
+      <c r="D4" s="19" t="s">
         <v>11</v>
       </c>
       <c r="E4" s="1"/>
@@ -1098,11 +1112,11 @@
     <row r="5" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
-      <c r="C5" s="20" t="s">
+      <c r="C5" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="21" t="s">
-        <v>26</v>
+      <c r="D5" s="19" t="s">
+        <v>21</v>
       </c>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
@@ -1111,10 +1125,10 @@
     <row r="6" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
-      <c r="C6" s="20" t="s">
+      <c r="C6" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="21" t="s">
+      <c r="D6" s="19" t="s">
         <v>12</v>
       </c>
       <c r="E6" s="1"/>
@@ -1124,53 +1138,53 @@
     <row r="7" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
-      <c r="C7" s="20" t="s">
+      <c r="C7" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="D7" s="21" t="s">
+      <c r="D7" s="19" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
-      <c r="C8" s="20" t="s">
+      <c r="C8" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="D8" s="21" t="s">
+      <c r="D8" s="19" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
-      <c r="C9" s="20" t="s">
+      <c r="C9" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="D9" s="21" t="s">
+      <c r="D9" s="19" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
-      <c r="C10" s="20" t="s">
+      <c r="C10" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="D10" s="21" t="s">
+      <c r="D10" s="19" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="185.25" x14ac:dyDescent="0.45">
-      <c r="C11" s="20" t="s">
+      <c r="C11" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="D11" s="22" t="s">
-        <v>24</v>
-      </c>
-      <c r="E11" s="19"/>
-      <c r="F11" s="19"/>
-      <c r="G11" s="19"/>
+      <c r="D11" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="E11" s="17"/>
+      <c r="F11" s="17"/>
+      <c r="G11" s="17"/>
     </row>
     <row r="12" spans="1:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A12" s="15"/>
@@ -1181,9 +1195,9 @@
       <c r="D12" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="E12" s="19"/>
-      <c r="F12" s="19"/>
-      <c r="G12" s="19"/>
+      <c r="E12" s="17"/>
+      <c r="F12" s="17"/>
+      <c r="G12" s="17"/>
     </row>
     <row r="13" spans="1:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="C13" s="1"/>
@@ -1205,7 +1219,7 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.45">
       <c r="C16" s="5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D16" s="9"/>
     </row>
@@ -1216,11 +1230,11 @@
       <c r="B17" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="C17" s="23" t="s">
-        <v>18</v>
+      <c r="C17" s="21" t="s">
+        <v>22</v>
       </c>
       <c r="D17" s="10" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
@@ -1229,21 +1243,66 @@
         <v>10</v>
       </c>
       <c r="C18" s="13" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="D18" s="14" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="C19" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="D19" s="18"/>
+      <c r="B19" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="C19" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="D19" s="16" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="C20" s="17"/>
-      <c r="D20" s="18"/>
+      <c r="B20" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="C20" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="D20" s="16" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B21" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="C21" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="D21" s="16" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B22" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="C22" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="D22" s="16" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B23" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="C23" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="D23" s="16" t="s">
+        <v>40</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>

</xml_diff>